<commit_message>
Updating MCC deposit accessions
</commit_message>
<xml_diff>
--- a/MCC_deposition_accessions.xlsx
+++ b/MCC_deposition_accessions.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{618C5C3A-164E-D540-BF8A-F6EACC6A3784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BenBeresford-Jones/Documents/PhD/MGBC/Manuscript/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17092052-A3D3-924D-A226-2CCE7F12F164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="940" windowWidth="27640" windowHeight="16080" xr2:uid="{4253E711-3A4C-C24C-B4A4-5F6C704E2936}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4253E711-3A4C-C24C-B4A4-5F6C704E2936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="157">
   <si>
     <t>Genome_ID</t>
   </si>
@@ -37,9 +42,6 @@
     <t>Strain_ID</t>
   </si>
   <si>
-    <t>Accession</t>
-  </si>
-  <si>
     <t>Genus</t>
   </si>
   <si>
@@ -485,13 +487,31 @@
   </si>
   <si>
     <t>C9</t>
+  </si>
+  <si>
+    <t>DSM number</t>
+  </si>
+  <si>
+    <t>MGBC000042</t>
+  </si>
+  <si>
+    <t>MGBC000032</t>
+  </si>
+  <si>
+    <t>MGBC000072</t>
+  </si>
+  <si>
+    <t>MGBC000073</t>
+  </si>
+  <si>
+    <t>MGBC000041</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -512,6 +532,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -620,21 +646,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,21 +993,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90BE376-4EAC-4F42-92B0-98F4F74A950B}">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:L98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -971,1014 +1016,1150 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="12">
+        <v>112781</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="C7" s="12"/>
       <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="5"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
+      <c r="C10" s="12"/>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="12"/>
+      <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="5"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5" t="s">
+      <c r="C15" s="12"/>
+      <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" t="s">
         <v>39</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5" t="s">
+      <c r="C18" s="15">
+        <v>112977</v>
+      </c>
+      <c r="D18" t="s">
         <v>41</v>
       </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="12">
+        <v>112986</v>
+      </c>
+      <c r="D20" t="s">
         <v>44</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="B21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="12"/>
       <c r="D21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="12">
+        <v>112987</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="D23" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" t="s">
         <v>51</v>
       </c>
-      <c r="D24" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" t="s">
         <v>53</v>
       </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" t="s">
         <v>55</v>
       </c>
-      <c r="D26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
-      <c r="B27" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="B27" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="12"/>
       <c r="D27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="B28" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="12"/>
       <c r="D28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="B29" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="B29" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="12"/>
       <c r="D29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" t="s">
         <v>60</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5" t="s">
-        <v>62</v>
+      <c r="C31" s="12">
+        <v>112780</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" t="s">
         <v>63</v>
       </c>
-      <c r="D32" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="6"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" t="s">
         <v>65</v>
       </c>
-      <c r="D33" t="s">
-        <v>66</v>
-      </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
-      <c r="B34" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="B34" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="12"/>
       <c r="D34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
-      <c r="B35" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="B35" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="12"/>
       <c r="D35" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="B36" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="12"/>
       <c r="D36" t="s">
-        <v>19</v>
-      </c>
-      <c r="E36" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="B37" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="12"/>
       <c r="D37" t="s">
-        <v>19</v>
-      </c>
-      <c r="E37" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="B38" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="12"/>
       <c r="D38" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" t="s">
         <v>72</v>
       </c>
-      <c r="D39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" t="s">
         <v>74</v>
       </c>
-      <c r="D40" t="s">
-        <v>75</v>
-      </c>
-      <c r="E40" s="6"/>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" t="s">
         <v>76</v>
       </c>
-      <c r="D41" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="6"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
-      <c r="B42" s="5" t="s">
-        <v>78</v>
-      </c>
+      <c r="B42" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="12"/>
       <c r="D42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E42" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" t="s">
         <v>79</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" t="s">
         <v>82</v>
       </c>
-      <c r="D44" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="6"/>
+      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
-      <c r="B45" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="B45" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="12"/>
       <c r="D45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E45" s="5"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
-      <c r="B46" s="5" t="s">
-        <v>85</v>
-      </c>
+      <c r="B46" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="12"/>
       <c r="D46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E46" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="E46" s="5"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
-      <c r="B47" s="5" t="s">
-        <v>86</v>
-      </c>
+      <c r="B47" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="12"/>
       <c r="D47" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
-      <c r="B48" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="B48" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="12"/>
       <c r="D48" t="s">
-        <v>64</v>
-      </c>
-      <c r="E48" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
-      <c r="B49" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="B49" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="12"/>
       <c r="D49" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
-      <c r="B50" s="5" t="s">
-        <v>89</v>
-      </c>
+      <c r="B50" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="12"/>
       <c r="D50" t="s">
-        <v>73</v>
-      </c>
-      <c r="E50" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
-      <c r="B51" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="B51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="12"/>
       <c r="D51" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
-      <c r="B52" s="5" t="s">
-        <v>91</v>
-      </c>
+      <c r="B52" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="12"/>
       <c r="D52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E52" s="5"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" t="s">
         <v>92</v>
       </c>
-      <c r="D53" t="s">
-        <v>93</v>
-      </c>
-      <c r="E53" s="6"/>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="12"/>
+      <c r="D54" t="s">
         <v>94</v>
       </c>
-      <c r="D54" t="s">
-        <v>95</v>
-      </c>
-      <c r="E54" s="6"/>
+      <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
-      <c r="B55" s="5" t="s">
-        <v>96</v>
-      </c>
+      <c r="B55" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="12"/>
       <c r="D55" t="s">
-        <v>61</v>
-      </c>
-      <c r="E55" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" t="s">
         <v>97</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
-      <c r="B57" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="B57" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="12"/>
       <c r="D57" t="s">
-        <v>38</v>
-      </c>
-      <c r="E57" s="6"/>
+        <v>37</v>
+      </c>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
-      <c r="B58" s="5" t="s">
-        <v>101</v>
-      </c>
+      <c r="B58" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="12"/>
       <c r="D58" t="s">
-        <v>61</v>
-      </c>
-      <c r="E58" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
-      <c r="B59" s="5" t="s">
-        <v>102</v>
-      </c>
+      <c r="B59" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="12"/>
       <c r="D59" t="s">
-        <v>19</v>
-      </c>
-      <c r="E59" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="4"/>
-      <c r="B60" s="5" t="s">
-        <v>103</v>
-      </c>
+      <c r="B60" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" s="12"/>
       <c r="D60" t="s">
-        <v>19</v>
-      </c>
-      <c r="E60" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="4"/>
-      <c r="B61" s="5" t="s">
-        <v>104</v>
-      </c>
+      <c r="B61" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" s="12"/>
       <c r="D61" t="s">
-        <v>19</v>
-      </c>
-      <c r="E61" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
-      <c r="B62" s="5" t="s">
-        <v>105</v>
-      </c>
+      <c r="B62" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C62" s="12"/>
       <c r="D62" t="s">
-        <v>19</v>
-      </c>
-      <c r="E62" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
-      <c r="B63" s="5" t="s">
-        <v>106</v>
-      </c>
+      <c r="B63" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="12"/>
       <c r="D63" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="12"/>
+      <c r="D64" t="s">
         <v>107</v>
       </c>
-      <c r="D64" t="s">
-        <v>108</v>
-      </c>
-      <c r="E64" s="6"/>
+      <c r="E64" s="5"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
-      <c r="B65" s="5" t="s">
-        <v>109</v>
-      </c>
+      <c r="B65" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="12"/>
       <c r="D65" t="s">
-        <v>93</v>
-      </c>
-      <c r="E65" s="6"/>
+        <v>92</v>
+      </c>
+      <c r="E65" s="5"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
-      <c r="B66" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="B66" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" s="12"/>
       <c r="D66" t="s">
-        <v>19</v>
-      </c>
-      <c r="E66" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E66" s="5"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="5" t="s">
-        <v>111</v>
-      </c>
+      <c r="B67" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C67" s="12"/>
       <c r="D67" t="s">
-        <v>19</v>
-      </c>
-      <c r="E67" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E67" s="5"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
-      <c r="B68" s="5" t="s">
-        <v>112</v>
-      </c>
+      <c r="B68" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" s="12"/>
       <c r="D68" t="s">
-        <v>19</v>
-      </c>
-      <c r="E68" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E68" s="5"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
-      <c r="B69" s="8" t="s">
+      <c r="B69" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C69" s="12"/>
+      <c r="D69" t="s">
         <v>113</v>
       </c>
-      <c r="D69" t="s">
-        <v>114</v>
-      </c>
-      <c r="E69" s="6"/>
+      <c r="E69" s="5"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
-      <c r="B70" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="B70" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C70" s="12"/>
       <c r="D70" t="s">
-        <v>73</v>
-      </c>
-      <c r="E70" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="E70" s="5"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
-      <c r="B71" s="5" t="s">
-        <v>116</v>
-      </c>
+      <c r="B71" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C71" s="12"/>
       <c r="D71" t="s">
-        <v>73</v>
-      </c>
-      <c r="E71" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="E71" s="5"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
-      <c r="B72" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="B72" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C72" s="12"/>
       <c r="D72" t="s">
-        <v>64</v>
-      </c>
-      <c r="E72" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="E72" s="5"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="4"/>
-      <c r="B73" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="B73" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C73" s="12"/>
       <c r="D73" t="s">
-        <v>61</v>
-      </c>
-      <c r="E73" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="E73" s="5"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="4"/>
-      <c r="B74" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="B74" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C74" s="12"/>
       <c r="D74" t="s">
-        <v>19</v>
-      </c>
-      <c r="E74" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E74" s="5"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" t="s">
+        <v>94</v>
+      </c>
+      <c r="E75" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="D75" t="s">
-        <v>95</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="4"/>
-      <c r="B76" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="B76" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" s="12"/>
       <c r="D76" t="s">
-        <v>19</v>
-      </c>
-      <c r="E76" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E76" s="5"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
-      <c r="B77" s="5" t="s">
-        <v>123</v>
-      </c>
+      <c r="B77" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77" s="12"/>
       <c r="D77" t="s">
-        <v>19</v>
-      </c>
-      <c r="E77" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E77" s="5"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
-      <c r="B78" s="8" t="s">
-        <v>124</v>
-      </c>
+      <c r="B78" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C78" s="12"/>
       <c r="D78" t="s">
-        <v>19</v>
-      </c>
-      <c r="E78" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E78" s="5"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
-      <c r="B79" s="5" t="s">
-        <v>125</v>
-      </c>
+      <c r="B79" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C79" s="12"/>
       <c r="D79" t="s">
-        <v>75</v>
-      </c>
-      <c r="E79" s="6"/>
+        <v>74</v>
+      </c>
+      <c r="E79" s="5"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
-      <c r="B80" s="5" t="s">
-        <v>126</v>
-      </c>
+      <c r="B80" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" s="12"/>
       <c r="D80" t="s">
-        <v>61</v>
-      </c>
-      <c r="E80" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="E80" s="5"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
-      <c r="B81" s="5" t="s">
-        <v>127</v>
-      </c>
+      <c r="B81" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="12"/>
       <c r="D81" t="s">
-        <v>12</v>
-      </c>
-      <c r="E81" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E81" s="5"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="4"/>
-      <c r="B82" s="5" t="s">
-        <v>128</v>
-      </c>
+      <c r="B82" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C82" s="12"/>
       <c r="D82" t="s">
-        <v>19</v>
-      </c>
-      <c r="E82" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E82" s="5"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="4"/>
-      <c r="B83" s="8" t="s">
+      <c r="B83" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C83" s="12"/>
+      <c r="D83" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="D83" t="s">
-        <v>21</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="4"/>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C84" s="12"/>
+      <c r="D84" t="s">
         <v>131</v>
       </c>
-      <c r="D84" t="s">
-        <v>132</v>
-      </c>
-      <c r="E84" s="6"/>
+      <c r="E84" s="5"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="4"/>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C85" s="12"/>
+      <c r="D85" t="s">
+        <v>20</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="D85" t="s">
-        <v>21</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="4"/>
-      <c r="B86" s="5" t="s">
-        <v>135</v>
-      </c>
+      <c r="B86" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C86" s="12"/>
       <c r="D86" t="s">
-        <v>77</v>
-      </c>
-      <c r="E86" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="E86" s="5"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="4"/>
-      <c r="B87" s="5" t="s">
-        <v>136</v>
-      </c>
+      <c r="B87" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C87" s="12"/>
       <c r="D87" t="s">
-        <v>61</v>
-      </c>
-      <c r="E87" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="E87" s="5"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="4"/>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88" s="12"/>
+      <c r="D88" t="s">
         <v>137</v>
       </c>
-      <c r="D88" t="s">
-        <v>138</v>
-      </c>
-      <c r="E88" s="6"/>
+      <c r="E88" s="5"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="4"/>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C89" s="12"/>
+      <c r="D89" t="s">
         <v>139</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="4"/>
-      <c r="B90" s="5" t="s">
-        <v>142</v>
-      </c>
+      <c r="B90" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C90" s="12"/>
       <c r="D90" t="s">
-        <v>24</v>
-      </c>
-      <c r="E90" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="E90" s="5"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="4"/>
-      <c r="B91" s="5" t="s">
-        <v>143</v>
-      </c>
+      <c r="B91" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91" s="12"/>
       <c r="D91" t="s">
-        <v>12</v>
-      </c>
-      <c r="E91" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E91" s="5"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="4"/>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C92" s="12"/>
+      <c r="D92" t="s">
         <v>144</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="4"/>
-      <c r="B93" s="5" t="s">
-        <v>104</v>
-      </c>
+      <c r="B93" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C93" s="12"/>
       <c r="D93" t="s">
-        <v>19</v>
-      </c>
-      <c r="E93" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E93" s="5"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
-      <c r="B94" s="5" t="s">
-        <v>147</v>
-      </c>
+      <c r="B94" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C94" s="12"/>
       <c r="D94" t="s">
-        <v>19</v>
-      </c>
-      <c r="E94" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E94" s="5"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
-      <c r="B95" s="5" t="s">
-        <v>148</v>
-      </c>
+      <c r="B95" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C95" s="12"/>
       <c r="D95" t="s">
-        <v>19</v>
-      </c>
-      <c r="E95" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E95" s="5"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
-      <c r="B96" s="5" t="s">
-        <v>149</v>
-      </c>
+      <c r="B96" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C96" s="12"/>
       <c r="D96" t="s">
-        <v>19</v>
-      </c>
-      <c r="E96" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="E96" s="5"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C97" s="12"/>
+      <c r="D97" t="s">
+        <v>60</v>
+      </c>
+      <c r="E97" s="5"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="7"/>
+      <c r="B98" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="D97" t="s">
-        <v>61</v>
-      </c>
-      <c r="E97" s="6"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="10"/>
-      <c r="B98" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E98" s="13"/>
+      <c r="C98" s="17"/>
+      <c r="D98" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating MCC deposition accessions
</commit_message>
<xml_diff>
--- a/MCC_deposition_accessions.xlsx
+++ b/MCC_deposition_accessions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BenBeresford-Jones/Documents/PhD/MGBC/Manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17092052-A3D3-924D-A226-2CCE7F12F164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBD85DD-4E54-AA4E-A8B5-83AA77A52B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4253E711-3A4C-C24C-B4A4-5F6C704E2936}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{4253E711-3A4C-C24C-B4A4-5F6C704E2936}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="159">
   <si>
     <t>Genome_ID</t>
   </si>
@@ -505,6 +505,12 @@
   </si>
   <si>
     <t>MGBC000041</t>
+  </si>
+  <si>
+    <t>MGBC000054</t>
+  </si>
+  <si>
+    <t>MGBC000029</t>
   </si>
 </sst>
 </file>
@@ -995,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90BE376-4EAC-4F42-92B0-98F4F74A950B}">
   <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,11 +1032,15 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
+      <c r="A2" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="12">
+        <v>112978</v>
+      </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
@@ -1677,11 +1687,15 @@
       <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
+      <c r="A56" s="4" t="s">
+        <v>158</v>
+      </c>
       <c r="B56" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="12"/>
+      <c r="C56" s="12">
+        <v>113311</v>
+      </c>
       <c r="D56" t="s">
         <v>97</v>
       </c>

</xml_diff>